<commit_message>
pola i typy na 19.04
</commit_message>
<xml_diff>
--- a/model_logiczny.xlsx
+++ b/model_logiczny.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s-121-24\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937FFF3A-284F-4410-91FB-000D66A1233D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD510205-DD29-4CCE-86DE-56F5039476DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19035" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabele" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
   <si>
     <t>Krotność</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Klucz obcy</t>
   </si>
   <si>
-    <t>tabela</t>
-  </si>
-  <si>
     <t>Zamówienie</t>
   </si>
   <si>
@@ -146,6 +143,66 @@
   </si>
   <si>
     <t>tabela podzbiór</t>
+  </si>
+  <si>
+    <t>cups_colors</t>
+  </si>
+  <si>
+    <t>tabela łącząca</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>int(liczba)</t>
+  </si>
+  <si>
+    <t>order_value</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>flavor</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>cup_id</t>
+  </si>
+  <si>
+    <t>color_id</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>color_name</t>
+  </si>
+  <si>
+    <t>varcahr(20)</t>
   </si>
 </sst>
 </file>
@@ -177,7 +234,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -200,21 +257,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -261,9 +363,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2007–2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -301,9 +403,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2007–2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -336,26 +438,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,26 +473,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2007–2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -583,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,64 +672,68 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -678,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,14 +790,14 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -733,14 +805,14 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -748,42 +820,60 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -799,47 +889,47 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -859,69 +949,409 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="C1:F47"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43:I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="7">
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C28:F28"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -936,7 +1366,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>